<commit_message>
Revised Reprocessing Works based on recycling flows (eg. OCC, ONP) not waste flows
</commit_message>
<xml_diff>
--- a/swolfpy/Data/Material properties - process modles.xlsx
+++ b/swolfpy/Data/Material properties - process modles.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msardar2\Google Drive\Brightway2\PySWOLF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msmsa\Google Drive\Brightway2\swolfpy\swolfpy\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B22B3C7-B15F-4E92-BE79-67AEC9E43777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="6"/>
+    <workbookView xWindow="-25310" yWindow="3030" windowWidth="25420" windowHeight="15370" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Composting" sheetId="1" r:id="rId1"/>
@@ -25,12 +26,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -890,7 +885,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1423,57 +1418,57 @@
     </xf>
   </cellXfs>
   <cellStyles count="51">
-    <cellStyle name="Currency 2" xfId="40"/>
-    <cellStyle name="Currency 3" xfId="26"/>
-    <cellStyle name="Hyperlink 2" xfId="32"/>
-    <cellStyle name="Hyperlink 3" xfId="27"/>
+    <cellStyle name="Currency 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Currency 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Hyperlink 3" xfId="27" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 2 2" xfId="6"/>
-    <cellStyle name="Normal 2 2 2" xfId="9"/>
-    <cellStyle name="Normal 2 2 3" xfId="12"/>
-    <cellStyle name="Normal 2 2 4" xfId="14"/>
-    <cellStyle name="Normal 2 2 5" xfId="17"/>
-    <cellStyle name="Normal 2 2 6" xfId="20"/>
-    <cellStyle name="Normal 2 2 7" xfId="23"/>
-    <cellStyle name="Normal 2 2 8" xfId="8"/>
-    <cellStyle name="Normal 2 3" xfId="11"/>
-    <cellStyle name="Normal 2 3 2" xfId="33"/>
-    <cellStyle name="Normal 2 4" xfId="10"/>
-    <cellStyle name="Normal 2 4 2" xfId="34"/>
-    <cellStyle name="Normal 2 5" xfId="16"/>
-    <cellStyle name="Normal 2 5 2" xfId="35"/>
-    <cellStyle name="Normal 2 6" xfId="19"/>
-    <cellStyle name="Normal 2 6 2" xfId="36"/>
-    <cellStyle name="Normal 2 7" xfId="22"/>
-    <cellStyle name="Normal 2 7 2" xfId="37"/>
-    <cellStyle name="Normal 3" xfId="18"/>
-    <cellStyle name="Normal 3 2" xfId="31"/>
-    <cellStyle name="Normal 3 2 2" xfId="44"/>
-    <cellStyle name="Normal 3 3" xfId="38"/>
-    <cellStyle name="Normal 4" xfId="24"/>
-    <cellStyle name="Normal 4 2" xfId="39"/>
-    <cellStyle name="Normal 5" xfId="13"/>
-    <cellStyle name="Normal 6" xfId="15"/>
-    <cellStyle name="Normal 6 2" xfId="46"/>
-    <cellStyle name="Normal 7" xfId="21"/>
-    <cellStyle name="Normal 8" xfId="2"/>
-    <cellStyle name="Normal 8 2" xfId="41"/>
-    <cellStyle name="Normal 8 2 2" xfId="50"/>
-    <cellStyle name="Normal 8 3" xfId="28"/>
-    <cellStyle name="Normal 8 4" xfId="47"/>
-    <cellStyle name="Normal 9" xfId="30"/>
-    <cellStyle name="Normal 9 2" xfId="43"/>
-    <cellStyle name="Normal 9 3" xfId="48"/>
-    <cellStyle name="Normal_changes" xfId="3"/>
-    <cellStyle name="Normal_MRF" xfId="45"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 2 3" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 2 4" xfId="14" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2 2 5" xfId="17" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 2 2 6" xfId="20" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 2 2 7" xfId="23" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 2 2 8" xfId="8" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2 3 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 2 4 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 2 5" xfId="16" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 2 5 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 2 6" xfId="19" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 2 6 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 2 7" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 2 7 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 3 3" xfId="38" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 4" xfId="24" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 4 2" xfId="39" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 5" xfId="13" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 6" xfId="15" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 6 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 7" xfId="21" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 8" xfId="2" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 8 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 8 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 8 3" xfId="28" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 8 4" xfId="47" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 9" xfId="30" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 9 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 9 3" xfId="48" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal_changes" xfId="3" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal_MRF" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="4"/>
-    <cellStyle name="Percent 2 2" xfId="7"/>
-    <cellStyle name="Percent 3" xfId="25"/>
-    <cellStyle name="Percent 3 2" xfId="42"/>
-    <cellStyle name="Percent 3 3" xfId="29"/>
-    <cellStyle name="Percent 3 4" xfId="49"/>
+    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Percent 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Percent 3" xfId="25" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Percent 3 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Percent 3 3" xfId="29" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Percent 3 4" xfId="49" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1750,25 +1745,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O1" sqref="L1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="25.5703125" style="19" customWidth="1"/>
-    <col min="12" max="15" width="25.5703125" style="54" customWidth="1"/>
-    <col min="16" max="17" width="25.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="25.54296875" style="19" customWidth="1"/>
+    <col min="12" max="15" width="25.54296875" style="54" customWidth="1"/>
+    <col min="16" max="17" width="25.54296875" style="19" customWidth="1"/>
     <col min="18" max="18" width="31" style="22" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="24" style="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="67" width="25.5703125" style="19" customWidth="1"/>
-    <col min="68" max="16384" width="9.140625" style="19"/>
+    <col min="20" max="67" width="25.54296875" style="19" customWidth="1"/>
+    <col min="68" max="16384" width="9.1796875" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="16" customFormat="1" ht="81" customHeight="1">
@@ -5013,19 +5008,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="31" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="20.85546875" style="19" customWidth="1"/>
-    <col min="10" max="13" width="25.5703125" style="54" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="19"/>
+    <col min="2" max="9" width="20.81640625" style="19" customWidth="1"/>
+    <col min="10" max="13" width="25.54296875" style="54" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="33" customFormat="1" ht="81" customHeight="1">
@@ -7374,30 +7369,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" style="54" customWidth="1"/>
-    <col min="2" max="2" width="52.42578125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.7265625" style="54" customWidth="1"/>
+    <col min="2" max="2" width="52.453125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" style="35" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="35"/>
+    <col min="11" max="11" width="28.7265625" style="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="43" customFormat="1" ht="60">
+    <row r="1" spans="1:16" s="43" customFormat="1" ht="58">
       <c r="A1" s="40" t="s">
         <v>94</v>
       </c>
@@ -8694,7 +8689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BS64"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -8703,59 +8698,59 @@
       <selection pane="bottomLeft" activeCell="E72" sqref="E71:E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" style="54" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" style="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.54296875" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.81640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.453125" style="54" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="54" customWidth="1"/>
     <col min="13" max="13" width="9" style="54" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="54"/>
+    <col min="14" max="14" width="9.1796875" style="54"/>
     <col min="15" max="15" width="9" style="54" bestFit="1" customWidth="1"/>
-    <col min="16" max="22" width="9.140625" style="54"/>
+    <col min="16" max="22" width="9.1796875" style="54"/>
     <col min="23" max="23" width="22" style="54" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="8.5703125" style="54" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="54"/>
-    <col min="29" max="29" width="8.5703125" style="54" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.7109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="8.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="9.140625" style="54"/>
-    <col min="36" max="36" width="8.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="8.54296875" style="54" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.1796875" style="54"/>
+    <col min="29" max="29" width="8.54296875" style="54" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.7265625" style="54" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="8.81640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="9.1796875" style="54"/>
+    <col min="36" max="36" width="8.81640625" style="54" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="9" style="54" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="10" style="54" bestFit="1" customWidth="1"/>
     <col min="39" max="41" width="9" style="54" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.140625" style="54"/>
-    <col min="43" max="43" width="9.5703125" style="54" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="9.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="9.140625" style="54"/>
-    <col min="50" max="50" width="9.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.140625" style="54"/>
+    <col min="42" max="42" width="9.1796875" style="54"/>
+    <col min="43" max="43" width="9.54296875" style="54" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.81640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="9.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="9.1796875" style="54"/>
+    <col min="50" max="50" width="9.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.1796875" style="54"/>
     <col min="52" max="52" width="10" style="54" bestFit="1" customWidth="1"/>
     <col min="53" max="55" width="9" style="54" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.140625" style="54"/>
-    <col min="57" max="57" width="9.5703125" style="54" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.1796875" style="54"/>
+    <col min="57" max="57" width="9.54296875" style="54" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="10" style="54" bestFit="1" customWidth="1"/>
-    <col min="59" max="64" width="9.140625" style="54"/>
+    <col min="59" max="64" width="9.1796875" style="54"/>
     <col min="65" max="65" width="9" style="54" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="10" style="54" bestFit="1" customWidth="1"/>
     <col min="67" max="69" width="9" style="54" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="9.140625" style="54"/>
-    <col min="71" max="71" width="9.5703125" style="54" bestFit="1" customWidth="1"/>
-    <col min="72" max="16384" width="9.140625" style="54"/>
+    <col min="70" max="70" width="9.1796875" style="54"/>
+    <col min="71" max="71" width="9.54296875" style="54" bestFit="1" customWidth="1"/>
+    <col min="72" max="16384" width="9.1796875" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" s="16" customFormat="1" ht="150">
+    <row r="1" spans="1:71" s="16" customFormat="1" ht="130.5">
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
@@ -9111,7 +9106,7 @@
       <c r="BR3" s="50"/>
       <c r="BS3" s="50"/>
     </row>
-    <row r="4" spans="1:71" ht="45">
+    <row r="4" spans="1:71" ht="29">
       <c r="A4" s="34" t="s">
         <v>82</v>
       </c>
@@ -14911,20 +14906,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" style="87" customWidth="1"/>
+    <col min="1" max="1" width="48.453125" style="87" customWidth="1"/>
     <col min="2" max="29" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="62" customFormat="1" ht="30">
+    <row r="1" spans="1:29" s="62" customFormat="1" ht="29">
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
@@ -15360,19 +15355,19 @@
       <c r="D12" s="60"/>
       <c r="E12" s="60"/>
       <c r="F12" s="60">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="G12" s="60">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="H12" s="60">
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="I12" s="60">
         <v>0</v>
       </c>
       <c r="J12" s="60">
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="K12" s="60">
         <v>0</v>
@@ -17129,20 +17124,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" customWidth="1"/>
-    <col min="2" max="30" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="50.81640625" customWidth="1"/>
+    <col min="2" max="30" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="65" customFormat="1" ht="30">
+    <row r="1" spans="1:30" s="65" customFormat="1" ht="29">
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
@@ -19428,20 +19423,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J12" sqref="F11:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" customWidth="1"/>
-    <col min="2" max="30" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="49.26953125" customWidth="1"/>
+    <col min="2" max="30" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="65" customFormat="1" ht="30">
+    <row r="1" spans="1:30" s="65" customFormat="1" ht="29">
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
@@ -19890,19 +19885,19 @@
       <c r="D12" s="75"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75">
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="G12" s="75">
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="H12" s="75">
-        <v>0.94</v>
+        <v>0</v>
       </c>
       <c r="I12" s="75">
         <v>0</v>
       </c>
       <c r="J12" s="75">
-        <v>0.94</v>
+        <v>0</v>
       </c>
       <c r="K12" s="75">
         <v>0</v>

</xml_diff>

<commit_message>
Remove uncertainty from WTE input data.
</commit_message>
<xml_diff>
--- a/swolfpy/Data/Material properties - process modles.xlsx
+++ b/swolfpy/Data/Material properties - process modles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msmsa\Google Drive\Brightway2\swolfpy\swolfpy\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B22B3C7-B15F-4E92-BE79-67AEC9E43777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283B3D0B-E61A-474F-A6F1-92F14B0ECDAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25310" yWindow="3030" windowWidth="25420" windowHeight="15370" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25310" yWindow="3030" windowWidth="25420" windowHeight="15370" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Composting" sheetId="1" r:id="rId1"/>
@@ -8692,10 +8692,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BS64"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="E72" sqref="E71:E72"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="J13:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -10355,15 +10355,9 @@
       <c r="I17" s="51">
         <v>1.3360000000000001</v>
       </c>
-      <c r="J17" s="51">
-        <v>3</v>
-      </c>
-      <c r="K17" s="51">
-        <v>1.3</v>
-      </c>
-      <c r="L17" s="51">
-        <v>0.3</v>
-      </c>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
       <c r="M17" s="51"/>
       <c r="N17" s="51"/>
       <c r="O17" s="51"/>
@@ -10447,22 +10441,12 @@
       <c r="B18" s="39">
         <v>1</v>
       </c>
-      <c r="C18" s="85">
-        <v>3</v>
-      </c>
-      <c r="D18" s="39">
-        <v>0.9</v>
-      </c>
-      <c r="E18" s="39">
-        <v>0.05</v>
-      </c>
+      <c r="C18" s="85"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="39"/>
-      <c r="G18" s="39">
-        <v>0.8</v>
-      </c>
-      <c r="H18" s="39">
-        <v>1</v>
-      </c>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
       <c r="I18" s="52">
         <v>1.3360000000000001</v>
       </c>
@@ -10742,34 +10726,18 @@
       <c r="B21" s="39">
         <v>1</v>
       </c>
-      <c r="C21" s="85">
-        <v>3</v>
-      </c>
-      <c r="D21" s="39">
-        <v>0.9</v>
-      </c>
-      <c r="E21" s="39">
-        <v>0.05</v>
-      </c>
+      <c r="C21" s="85"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="39"/>
-      <c r="G21" s="39">
-        <v>0.8</v>
-      </c>
-      <c r="H21" s="39">
-        <v>1</v>
-      </c>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
       <c r="I21" s="51">
         <v>1.3360000000000001</v>
       </c>
-      <c r="J21" s="51">
-        <v>3</v>
-      </c>
-      <c r="K21" s="51">
-        <v>1.3</v>
-      </c>
-      <c r="L21" s="51">
-        <v>0.3</v>
-      </c>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
       <c r="M21" s="51"/>
       <c r="N21" s="51"/>
       <c r="O21" s="51"/>
@@ -14909,7 +14877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>

</xml_diff>